<commit_message>
new coding assignment for james
</commit_message>
<xml_diff>
--- a/docs/coding_scheme.xlsx
+++ b/docs/coding_scheme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Documents\Academics\1-Projects\HowisonLab\softcite\softcite-kb-cord19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Documents\Academics\1-Projects\HowisonLab\softcite\softcite-kb-cord19\cord19-sw-analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC913EBD-1C52-4DAE-970D-DF8A526BC127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D301DF0-5F2C-408D-A39B-E35151C7019B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C526BB6-DACE-46F1-AAD1-70F4CC0E98DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
   <si>
     <t>coding_scheme</t>
   </si>
@@ -420,9 +420,6 @@
     <t>This might include publications that merely discusses algorithms/methods even as computational procedures, but not a concrete code product. For instance, publications in computer science or bioinformatics commonly discuss algorithms or programming methods.</t>
   </si>
   <si>
-    <t>Paste the reference string from the publication if the extracted one is not correct (otherwise leaves the cell empty):</t>
-  </si>
-  <si>
     <t>B8-B11 are included to understand reference as part of the software mention and whether the reference provides additional information about the software mentioned in text.</t>
   </si>
   <si>
@@ -468,10 +465,6 @@
     <t>The citation request asks to cite the software itself.</t>
   </si>
   <si>
-    <t>This code requires finding the citation request online if available. 
-Any public information that address how to cite the software from the official source of the software (i.e. not a third party) is interpreted as a citation request. (i.e., it may not contain phrase like "request" but specify a way to reference the software)</t>
-  </si>
-  <si>
     <t>explanation</t>
   </si>
   <si>
@@ -481,9 +474,6 @@
     <t>The citation request asks to cite a "software publication" or a publication that discuss the software as the primary subject matter.</t>
   </si>
   <si>
-    <t>The citation request asks to a domain science publication.</t>
-  </si>
-  <si>
     <t>See the explanation for B3.</t>
   </si>
   <si>
@@ -506,11 +496,6 @@
   </si>
   <si>
     <t>The software has at least one version published to an archival repository (e.g., Zenodo, figshare, Software Heritage)</t>
-  </si>
-  <si>
-    <t>Web search using "&lt;software name&gt;"+"DOI" OR "&lt;software name&gt;"+"figshare" OR "&lt;software name&gt;"+"software heritage" to locate if an archival copy of the software (no matter which version) exists.
- If a general Web search of the mentioned software has an archival copy in an institutional repository in the search engine results page, then this code is also TRUE.
-If you identify any archival copy of the mentioned software during the search process, then this code is TRUE.</t>
   </si>
   <si>
     <t>The software has at least one version that has a unique and persistent identifier such as a DOI, ARK, Handle, PURL, or NBN.</t>
@@ -531,6 +516,24 @@
   </si>
   <si>
     <t>OPTIONAL please copy and paste the link to the software metadata:</t>
+  </si>
+  <si>
+    <t>Paste the reference string from the publication if the extracted one is not correct (otherwise leave the cell empty):</t>
+  </si>
+  <si>
+    <t>Web search using "&lt;software name&gt;"+"Zenodo" OR "&lt;software name&gt;"+"figshare" OR "&lt;software name&gt;"+"software heritage" to locate if an archival copy of the software (no matter which version) exists.
+ If a general Web search of the mentioned software has an archival copy in an institutional repository in the search engine results page, then this code is also TRUE.
+If you identify any archival copy of the mentioned software during the search process, then this code is TRUE.</t>
+  </si>
+  <si>
+    <t>The citation request asks to cite a domain science publication.</t>
+  </si>
+  <si>
+    <t>This code requires finding the citation request online if available. 
+Any public information that address how to cite the software from the official source of the software (i.e. not a third party) is interpreted as a citation request. (i.e., it may not contain phrase like "request" but specify a way to reference the software). If a citation request is not available, code D1 through to D14 as "0".</t>
+  </si>
+  <si>
+    <t>publish software</t>
   </si>
 </sst>
 </file>
@@ -960,9 +963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5DA6A6-467B-41FD-B927-35764C8A1222}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>23</v>
@@ -1221,7 +1224,7 @@
         <v>121</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -1326,7 +1329,7 @@
         <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
@@ -1343,7 +1346,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="8"/>
@@ -1385,7 +1388,7 @@
     <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>15</v>
@@ -1403,13 +1406,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="5" t="s">
@@ -1424,7 +1427,7 @@
         <v>79</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="4"/>
@@ -1440,7 +1443,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="4"/>
@@ -1469,7 +1472,7 @@
         <v>82</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="8"/>
@@ -1490,7 +1493,7 @@
         <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="5" t="s">
@@ -1523,7 +1526,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
@@ -1572,7 +1575,7 @@
       <c r="G37" s="3"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -1580,10 +1583,10 @@
         <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
@@ -1623,7 +1626,7 @@
         <v>92</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="8"/>
@@ -1637,10 +1640,10 @@
         <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="3"/>
@@ -1711,7 +1714,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="8"/>
@@ -1727,10 +1730,10 @@
         <v>99</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="3"/>
@@ -1745,10 +1748,10 @@
         <v>100</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="3"/>
@@ -1761,10 +1764,10 @@
         <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="3"/>
@@ -1777,7 +1780,7 @@
         <v>102</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="8"/>
@@ -1791,7 +1794,7 @@
         <v>103</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
@@ -1805,7 +1808,7 @@
         <v>104</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
@@ -1814,15 +1817,17 @@
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" ht="174" x14ac:dyDescent="0.35">
-      <c r="A54" s="3"/>
+      <c r="A54" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="B54" s="11" t="s">
         <v>105</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E54" s="8"/>
       <c r="G54" s="6"/>
@@ -1834,10 +1839,10 @@
         <v>106</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E55" s="8"/>
       <c r="G55" s="6"/>
@@ -1851,10 +1856,10 @@
         <v>107</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E56" s="3"/>
       <c r="G56" s="6"/>
@@ -1865,10 +1870,10 @@
     <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E57" s="3"/>
     </row>

</xml_diff>

<commit_message>
update coding scheme for consistency
</commit_message>
<xml_diff>
--- a/docs/coding_scheme.xlsx
+++ b/docs/coding_scheme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Documents\Academics\1-Projects\HowisonLab\softcite\softcite-kb-cord19\cord19-sw-analysis\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Documents\Academics\1-Projects\HowisonLab\softcite\softcite-kb-cord19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B295A-E2C8-4C27-A136-675EB5FF9BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB0424E-2DCC-4A49-A6A9-CC6991909713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C526BB6-DACE-46F1-AAD1-70F4CC0E98DB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="170">
   <si>
     <t>coding_scheme</t>
   </si>
@@ -456,9 +456,6 @@
     <t>This might include publications that merely discuss algorithms/methods even as computational procedures, but not a concrete code product. For instance, publications in computer science or bioinformatics commonly discuss algorithms or programming methods.</t>
   </si>
   <si>
-    <t>A specific computational product that needs to be instantiated by code to realize the reported research in the publication. Examples include specific computational models or algorithms that are implemented according to the context. Exceptions include a general analysis method being mentioned but is not necessarily implemented by some form of code.</t>
-  </si>
-  <si>
     <t>Paste the reference string from the publication if the extracted one is not correct (otherwise leave the cell empty or code as "0"):</t>
   </si>
   <si>
@@ -475,9 +472,6 @@
   </si>
   <si>
     <t>B9-B12 are included to understand reference as part of the software mention and whether the reference provides additional information about the software mentioned in text.</t>
-  </si>
-  <si>
-    <t>The software has at least one findable official presence (e.g., source code, online manual, or an online resource such as a metadata record or webpage that is dedicated to the software).</t>
   </si>
   <si>
     <t>Use available information in in-text mention and references to search for the software for available online records.</t>
@@ -491,10 +485,6 @@
   </si>
   <si>
     <t>The citation request asks to cite a "software publication" or a publication that discusses the software as the primary subject matter.</t>
-  </si>
-  <si>
-    <t>Conduct a within-site search on Zenodo, Figshare, or Software Heritage using the software name plus possible keywords as search term. If an archival copy of the software (no matter which version) is found, then this code is TRUE.
-Also examine the web search results when searching for the specific piece of software using possible search terms. If an archival copy in an institutional repository or in locations mentioned above is located in the search engine results page, then this code is also TRUE.</t>
   </si>
   <si>
     <t>Web search using "&lt;software name&gt;"+"DOI" OR "&lt;software name&gt;"+"ARK" OR "&lt;software name&gt;"+"Handle" OR "&lt;software name&gt;"+"PURL" OR "&lt;software name&gt;"+"NBN" to locate if an archival copy of the software (no matter which version) exists.
@@ -542,6 +532,22 @@
   </si>
   <si>
     <t>If a CITATION/CITATION.cff/CodeMeta/R DESCRIPTION/R CITATION file exists and is populated with metadata items that describe the mentioned software, then this code is TRUE. The metadata could also be in a language specific form or any general software metadata form other than the citation-purpose metadata.</t>
+  </si>
+  <si>
+    <t>Conduct a within-site search on Zenodo, Figshare, or Software Heritage using the software name plus possible keywords as search term. If an archival copy of the software (no matter which version) is found, then this code is TRUE. Using the link of identified working repository for searching inside Software Heritage is particularly helpful.
+Also examine the web search results when searching for the specific piece of software using possible search terms. If an archival copy in an institutional repository or in locations mentioned above is located in the search engine results page, then this code is also TRUE.</t>
+  </si>
+  <si>
+    <t>A specific computational product that needs to be instantiated by code to realize the reported research in the publication. Examples include specific computational models or algorithms that are implemented according to the context. Exceptions include a general analysis method being mentioned but is not necessarily implemented by some form of code. If the extracted context does not mention software, then code all the rest codes as "0".</t>
+  </si>
+  <si>
+    <t>Use available information in in-text mention and references to search for the software for available online records. If no version is mentioned in the extracted texts, then code C3 as FALSE.</t>
+  </si>
+  <si>
+    <t>The software has at least one findable official presence (e.g., source code, online manual, publication, or an online resource such as a metadata record or webpage that is dedicated to the software).</t>
+  </si>
+  <si>
+    <t>Usually if the reference is a "software publication" or discusses the software substantially, the authors are counted as publishers/creators of the software.</t>
   </si>
 </sst>
 </file>
@@ -972,8 +978,8 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,7 +1015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
@@ -1325,7 +1331,7 @@
         <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="4"/>
@@ -1339,7 +1345,7 @@
         <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
@@ -1353,10 +1359,10 @@
         <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="8"/>
@@ -1369,7 +1375,7 @@
         <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="4"/>
@@ -1385,7 +1391,7 @@
         <v>66</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
@@ -1395,15 +1401,17 @@
       <c r="G25" s="6"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="11" t="s">
         <v>113</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>144</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="5" t="s">
         <v>35</v>
@@ -1431,16 +1439,16 @@
       <c r="G27" s="6"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="5" t="s">
@@ -1455,10 +1463,10 @@
         <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="8" t="s">
@@ -1525,7 +1533,7 @@
         <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="5" t="s">
@@ -1542,7 +1550,7 @@
         <v>16</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
@@ -1583,7 +1591,7 @@
         <v>76</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="4"/>
@@ -1599,10 +1607,10 @@
         <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
@@ -1615,7 +1623,7 @@
         <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="8"/>
@@ -1628,7 +1636,7 @@
         <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="8"/>
@@ -1672,7 +1680,7 @@
         <v>82</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="8"/>
@@ -1686,7 +1694,7 @@
         <v>83</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="8"/>
@@ -1700,7 +1708,7 @@
         <v>84</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="8"/>
@@ -1714,7 +1722,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="8"/>
@@ -1746,7 +1754,7 @@
         <v>87</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>124</v>
@@ -1832,7 +1840,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>135</v>
       </c>
@@ -1840,10 +1848,10 @@
         <v>93</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="E54" s="8"/>
       <c r="G54" s="6"/>
@@ -1858,7 +1866,7 @@
         <v>131</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E55" s="8"/>
       <c r="G55" s="6"/>
@@ -1872,10 +1880,10 @@
         <v>95</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E56" s="3"/>
       <c r="G56" s="6"/>

</xml_diff>

<commit_message>
getting things in order
</commit_message>
<xml_diff>
--- a/docs/coding_scheme.xlsx
+++ b/docs/coding_scheme.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Documents\Academics\1-Projects\HowisonLab\softcite\softcite-kb-cord19\cord19-sw-analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87439CA7-E496-4CB4-BD37-0E23F6A94C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01B7BE3-8B41-4F49-8ACC-55C6218CDAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C526BB6-DACE-46F1-AAD1-70F4CC0E98DB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3C526BB6-DACE-46F1-AAD1-70F4CC0E98DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="simplified" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="170">
-  <si>
-    <t>coding_scheme</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="286">
   <si>
     <t>Check `software_name`</t>
   </si>
@@ -313,9 +312,6 @@
   </si>
   <si>
     <t>D16</t>
-  </si>
-  <si>
-    <t>coding_id</t>
   </si>
   <si>
     <t>Either or both in-text mention and references contains a unique, persistent identifier (e.g., DOI, ARK, Handle, PURL, NBN) that can resolve to the software itself and/or its metadata. (i.e., the software itself is registered with a persistent URI)</t>
@@ -548,13 +544,370 @@
   </si>
   <si>
     <t>E4</t>
+  </si>
+  <si>
+    <t>Coding id</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>"Like instrument" mention</t>
+  </si>
+  <si>
+    <t>Software name</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>e.g., …were performed using the Prism 3.0 software (GraphPad Software, San Diego, CA, USA)</t>
+  </si>
+  <si>
+    <t>Software configuration details</t>
+  </si>
+  <si>
+    <t>e.g., operation environment; parameter settings</t>
+  </si>
+  <si>
+    <t>Cite to software publication</t>
+  </si>
+  <si>
+    <t>A "software publication" or a publication substantially discusses the technical aspects of the software</t>
+  </si>
+  <si>
+    <t>Cite to software</t>
+  </si>
+  <si>
+    <t>The software itself, instead of any publications, is referenced in bibliography</t>
+  </si>
+  <si>
+    <t>Cite to domain publication</t>
+  </si>
+  <si>
+    <t>A publication that discusses domain science topics, including methods or models but not their software instantiation</t>
+  </si>
+  <si>
+    <t>Cite to user manual/guide</t>
+  </si>
+  <si>
+    <t>Cite to a project</t>
+  </si>
+  <si>
+    <t>The documentation of the software is referenced</t>
+  </si>
+  <si>
+    <t>A project name or website is referenced</t>
+  </si>
+  <si>
+    <t>The name of the mentioned software is mentioned</t>
+  </si>
+  <si>
+    <t>Specific version number or release date is mentioned</t>
+  </si>
+  <si>
+    <t>Publisher or creator of software mentioned</t>
+  </si>
+  <si>
+    <t>Identifiable</t>
+  </si>
+  <si>
+    <t>The mention/citation enables identifying the software as a distinct identity (e.g., with a unique name; online information available from reliable sources)</t>
+  </si>
+  <si>
+    <t>Findable</t>
+  </si>
+  <si>
+    <t>Findable version</t>
+  </si>
+  <si>
+    <t>A stable presence of the mentioned software version can be found online.</t>
+  </si>
+  <si>
+    <t>A stable presence of the software in any relevant form (e.g., website; downloads; working repositories; documentation) can be found online.</t>
+  </si>
+  <si>
+    <t>Unique and persistent identifier</t>
+  </si>
+  <si>
+    <t>Referenced with unique and persistent identifier</t>
+  </si>
+  <si>
+    <t>Referenced with a commit hash</t>
+  </si>
+  <si>
+    <t>A possible form of unique and persistent identifier such as DOI, SWHID, ARK, Handle, NBN, or PURL is referenced as the software itself</t>
+  </si>
+  <si>
+    <t>A git commit hash is referenced for a snapshot of software</t>
+  </si>
+  <si>
+    <t>No access</t>
+  </si>
+  <si>
+    <t>No findable information online about how to access the software</t>
+  </si>
+  <si>
+    <t>Proprietary</t>
+  </si>
+  <si>
+    <t>A license fee has to be paid for accessing the software</t>
+  </si>
+  <si>
+    <t>Free access</t>
+  </si>
+  <si>
+    <t>Software can be accessed without a payment</t>
+  </si>
+  <si>
+    <t>Source code accessible</t>
+  </si>
+  <si>
+    <t>The source code of the software is available online</t>
+  </si>
+  <si>
+    <t>Permission to modify</t>
+  </si>
+  <si>
+    <t>The publisher has given permission to users for modifying the software (e.g., open source licensed or public domain software)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open source </t>
+  </si>
+  <si>
+    <t>The software has a standard open source license</t>
+  </si>
+  <si>
+    <t>Matches citation request</t>
+  </si>
+  <si>
+    <t>The software is mentioned in a way that matches the citation request by its publisher</t>
+  </si>
+  <si>
+    <t>Plain text citation request</t>
+  </si>
+  <si>
+    <t>The publisher has requested preferred citation in plain text style</t>
+  </si>
+  <si>
+    <t>BibTex citation request</t>
+  </si>
+  <si>
+    <t>The publisher has provided a preferred citation in BibTex format</t>
+  </si>
+  <si>
+    <t>Citation request in repository README</t>
+  </si>
+  <si>
+    <t>The publisher has requested preferred citation in the README of a working repository (e.g., on GitHub/GitLab)</t>
+  </si>
+  <si>
+    <t>Citation request on web page</t>
+  </si>
+  <si>
+    <t>The publisher has requested preferred citation on a webpage (e.g., project website; on a software catalog page)</t>
+  </si>
+  <si>
+    <t>CITATION file</t>
+  </si>
+  <si>
+    <t>A CITATION file is provided for requesting preferred citation</t>
+  </si>
+  <si>
+    <t>A CITATION.cff file is provided for requesting preferred citation</t>
+  </si>
+  <si>
+    <t>CITATION.cff</t>
+  </si>
+  <si>
+    <t>CodeMeta</t>
+  </si>
+  <si>
+    <t>A CodeMeta file is provided for requesting preferred citation</t>
+  </si>
+  <si>
+    <t>Domain-specific citation metadata</t>
+  </si>
+  <si>
+    <t>Domain-specifc citation metadata is provided such as a R CITATION/DESCRIPTION file</t>
+  </si>
+  <si>
+    <t>Request to cite software</t>
+  </si>
+  <si>
+    <t>The software publisher requests to cite the software itself</t>
+  </si>
+  <si>
+    <t>Request to cite software publication</t>
+  </si>
+  <si>
+    <t>The software publisher requests to cite a software publication</t>
+  </si>
+  <si>
+    <t>Request to cite domain publication</t>
+  </si>
+  <si>
+    <t>The software publisher requests to cite a domain science publication</t>
+  </si>
+  <si>
+    <t>Request to cite a project</t>
+  </si>
+  <si>
+    <t>The software publisher requests to cite a project rather than a software product</t>
+  </si>
+  <si>
+    <t>Request to cite other research product</t>
+  </si>
+  <si>
+    <t>The software publisher requests to cite other non-software products such as dataset</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>The software has at least one version archived in a archival repository (e.g., Zenodo; Figshare; institutional repository)</t>
+  </si>
+  <si>
+    <t>The software itself has a unique and persistent identifier (e.g., DOI, Handle, ARK, NBN, PURL, SWHID)</t>
+  </si>
+  <si>
+    <t>Metadata available</t>
+  </si>
+  <si>
+    <t>The software has publicly accessible metadata, including both citation metadata and package metadata</t>
+  </si>
+  <si>
+    <t>Software mention</t>
+  </si>
+  <si>
+    <t>Software reference</t>
+  </si>
+  <si>
+    <t>Citation function</t>
+  </si>
+  <si>
+    <t>Software access</t>
+  </si>
+  <si>
+    <t>Standard compliance</t>
+  </si>
+  <si>
+    <t>Themes</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>A web link mentioned in text with software (a resolvable identifier is counted)</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>Howison &amp; Bullard
+(2016)</t>
+  </si>
+  <si>
+    <t>Katz et al. (2019)</t>
+  </si>
+  <si>
+    <t>Smith et al.
+ (2016)</t>
+  </si>
+  <si>
+    <t>FAIR4RS
+(2021)</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>Check the extracted software name.</t>
+  </si>
+  <si>
+    <t>Check the extracted version.</t>
+  </si>
+  <si>
+    <t>Check the extracted publisher.</t>
+  </si>
+  <si>
+    <t>Check the extracted URL.</t>
+  </si>
+  <si>
+    <t>Check the extracted mention context.</t>
+  </si>
+  <si>
+    <t>Check the extracted reference.</t>
+  </si>
+  <si>
+    <t>Citation functions.</t>
+  </si>
+  <si>
+    <t>Access to software.</t>
+  </si>
+  <si>
+    <t>Citation request.</t>
+  </si>
+  <si>
+    <t>Publish software.</t>
+  </si>
+  <si>
+    <t>Hint</t>
+  </si>
+  <si>
+    <t>Codes</t>
+  </si>
+  <si>
+    <t>Code ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,6 +921,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -608,7 +979,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -616,11 +987,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -655,11 +1166,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,9 +1602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5DA6A6-467B-41FD-B927-35764C8A1222}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A1:H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -994,39 +1619,39 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="11" t="s">
-        <v>93</v>
+        <v>168</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
@@ -1036,13 +1661,13 @@
     <row r="3" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
@@ -1051,18 +1676,18 @@
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="2"/>
@@ -1070,13 +1695,13 @@
     <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
@@ -1085,18 +1710,18 @@
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="2"/>
@@ -1104,10 +1729,10 @@
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
@@ -1117,18 +1742,18 @@
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="2"/>
@@ -1136,10 +1761,10 @@
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4"/>
@@ -1149,13 +1774,13 @@
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
@@ -1166,28 +1791,28 @@
     <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4"/>
       <c r="F11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
@@ -1196,51 +1821,51 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
-        <v>36</v>
+      <c r="A13" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -1249,13 +1874,13 @@
     </row>
     <row r="16" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -1264,17 +1889,17 @@
     </row>
     <row r="17" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="2"/>
@@ -1282,10 +1907,10 @@
     <row r="18" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
@@ -1296,13 +1921,13 @@
     <row r="19" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="8"/>
@@ -1312,15 +1937,15 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="4"/>
       <c r="F20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="2"/>
@@ -1328,10 +1953,10 @@
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="4"/>
@@ -1342,10 +1967,10 @@
     <row r="22" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
@@ -1356,13 +1981,13 @@
     <row r="23" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="8"/>
@@ -1372,15 +1997,15 @@
     <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="4"/>
       <c r="F24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="2"/>
@@ -1388,15 +2013,15 @@
     <row r="25" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
       <c r="F25" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="2"/>
@@ -1404,37 +2029,37 @@
     <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="2"/>
@@ -1442,17 +2067,17 @@
     <row r="28" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="2"/>
@@ -1460,27 +2085,27 @@
     <row r="29" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B30" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="8"/>
@@ -1491,35 +2116,35 @@
     <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="8"/>
       <c r="F31" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="2"/>
@@ -1527,30 +2152,30 @@
     <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="B34" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
@@ -1560,10 +2185,10 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="4"/>
@@ -1574,10 +2199,10 @@
     <row r="36" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="4"/>
@@ -1588,10 +2213,10 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="4"/>
@@ -1601,16 +2226,16 @@
     </row>
     <row r="38" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
@@ -1620,10 +2245,10 @@
     <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="8"/>
@@ -1633,10 +2258,10 @@
     </row>
     <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B40" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="8"/>
@@ -1647,10 +2272,10 @@
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="8"/>
@@ -1661,13 +2286,13 @@
     <row r="42" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="3"/>
@@ -1677,10 +2302,10 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="8"/>
@@ -1691,10 +2316,10 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="8"/>
@@ -1705,10 +2330,10 @@
     <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="8"/>
@@ -1719,63 +2344,63 @@
     <row r="46" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="8"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="8"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="3"/>
@@ -1785,13 +2410,13 @@
     <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="3"/>
@@ -1801,10 +2426,10 @@
     <row r="51" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="8"/>
@@ -1815,10 +2440,10 @@
     <row r="52" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
@@ -1829,10 +2454,10 @@
     <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
@@ -1842,16 +2467,16 @@
     </row>
     <row r="54" spans="1:8" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E54" s="8"/>
       <c r="G54" s="6"/>
@@ -1860,44 +2485,44 @@
     <row r="55" spans="1:8" ht="203" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E55" s="8"/>
       <c r="G55" s="6"/>
       <c r="H55" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E56" s="3"/>
       <c r="G56" s="6"/>
       <c r="H56" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E57" s="3"/>
     </row>
@@ -1912,4 +2537,1499 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8691B96-1F8F-482E-8F3C-9D33E1778F0C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:D57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="112" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A9" s="46"/>
+      <c r="B9" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A11" s="46"/>
+      <c r="B11" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" ht="56" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="48"/>
+    </row>
+    <row r="13" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A13" s="49"/>
+      <c r="B13" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="48"/>
+    </row>
+    <row r="14" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A14" s="50"/>
+      <c r="B14" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="48"/>
+    </row>
+    <row r="15" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="98" x14ac:dyDescent="0.35">
+      <c r="A16" s="51"/>
+      <c r="B16" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="56" x14ac:dyDescent="0.35">
+      <c r="A17" s="51"/>
+      <c r="B17" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="70" x14ac:dyDescent="0.35">
+      <c r="A18" s="46"/>
+      <c r="B18" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="1:4" ht="70" x14ac:dyDescent="0.35">
+      <c r="A19" s="46"/>
+      <c r="B19" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A20" s="46"/>
+      <c r="B20" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="48"/>
+    </row>
+    <row r="21" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="48"/>
+    </row>
+    <row r="22" spans="1:4" ht="56.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="52"/>
+    </row>
+    <row r="23" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A23" s="46"/>
+      <c r="B23" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="48"/>
+    </row>
+    <row r="25" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="48"/>
+    </row>
+    <row r="26" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A26" s="46"/>
+      <c r="B26" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A27" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="84.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="84.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="46"/>
+      <c r="B29" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="98.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="51"/>
+      <c r="B30" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="52"/>
+    </row>
+    <row r="31" spans="1:4" ht="42.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="52"/>
+    </row>
+    <row r="32" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A32" s="46" t="s">
+        <v>280</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A33" s="46"/>
+      <c r="B33" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="56" x14ac:dyDescent="0.35">
+      <c r="A34" s="51"/>
+      <c r="B34" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A35" s="46"/>
+      <c r="B35" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="48"/>
+    </row>
+    <row r="36" spans="1:4" ht="70" x14ac:dyDescent="0.35">
+      <c r="A36" s="46"/>
+      <c r="B36" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="48"/>
+    </row>
+    <row r="37" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A37" s="46"/>
+      <c r="B37" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" s="48"/>
+    </row>
+    <row r="38" spans="1:4" ht="112" x14ac:dyDescent="0.35">
+      <c r="A38" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A39" s="46"/>
+      <c r="B39" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="48"/>
+    </row>
+    <row r="40" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A40" s="51"/>
+      <c r="B40" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="48"/>
+    </row>
+    <row r="41" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A41" s="46"/>
+      <c r="B41" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="48"/>
+    </row>
+    <row r="42" spans="1:4" ht="56" x14ac:dyDescent="0.35">
+      <c r="A42" s="46"/>
+      <c r="B42" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A43" s="46"/>
+      <c r="B43" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" s="48"/>
+    </row>
+    <row r="44" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A44" s="46"/>
+      <c r="B44" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="48"/>
+    </row>
+    <row r="45" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A45" s="46"/>
+      <c r="B45" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="48"/>
+    </row>
+    <row r="46" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A46" s="46"/>
+      <c r="B46" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="48"/>
+    </row>
+    <row r="47" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A47" s="46"/>
+      <c r="B47" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="48"/>
+    </row>
+    <row r="48" spans="1:4" ht="56" x14ac:dyDescent="0.35">
+      <c r="A48" s="46"/>
+      <c r="B48" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A49" s="46"/>
+      <c r="B49" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A50" s="46"/>
+      <c r="B50" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A51" s="46"/>
+      <c r="B51" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="48"/>
+    </row>
+    <row r="52" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A52" s="46"/>
+      <c r="B52" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" s="53"/>
+    </row>
+    <row r="53" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A53" s="46"/>
+      <c r="B53" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="53"/>
+    </row>
+    <row r="54" spans="1:4" ht="154" x14ac:dyDescent="0.35">
+      <c r="A54" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" s="48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="182" x14ac:dyDescent="0.35">
+      <c r="A55" s="46"/>
+      <c r="B55" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" s="48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+      <c r="A56" s="46"/>
+      <c r="B56" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A57" s="46"/>
+      <c r="B57" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:A14"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03EAC4A4-F5EF-43CC-9A24-94DEE25DD0D4}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.08984375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="45"/>
+      <c r="D1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="43"/>
+      <c r="B3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="43"/>
+      <c r="B4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
+      <c r="B5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="43"/>
+      <c r="B6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="43"/>
+      <c r="B7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="F7" s="34"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="43"/>
+      <c r="B9" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="43"/>
+      <c r="B10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="43"/>
+      <c r="B11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="43"/>
+      <c r="B12" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="31"/>
+    </row>
+    <row r="13" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="43"/>
+      <c r="B14" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="43"/>
+      <c r="B15" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="43"/>
+      <c r="B16" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="43"/>
+      <c r="B17" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="43"/>
+      <c r="B19" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="43"/>
+      <c r="B20" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="43"/>
+      <c r="B21" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H21" s="24"/>
+    </row>
+    <row r="22" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="43"/>
+      <c r="B22" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="43"/>
+      <c r="B23" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E23" s="34"/>
+      <c r="F23" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="43"/>
+      <c r="B25" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="43"/>
+      <c r="B26" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="43"/>
+      <c r="B27" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="43"/>
+      <c r="B28" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="43"/>
+      <c r="B29" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="E29" s="28"/>
+      <c r="F29" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H29" s="24"/>
+    </row>
+    <row r="30" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="43"/>
+      <c r="B30" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" s="28"/>
+      <c r="F30" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="43"/>
+      <c r="B31" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="E31" s="28"/>
+      <c r="F31" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="43"/>
+      <c r="B32" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="43"/>
+      <c r="B33" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H33" s="24"/>
+    </row>
+    <row r="34" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="43"/>
+      <c r="B34" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="24"/>
+    </row>
+    <row r="35" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="43"/>
+      <c r="B35" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="24"/>
+    </row>
+    <row r="36" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="43"/>
+      <c r="B36" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="24"/>
+    </row>
+    <row r="37" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="43"/>
+      <c r="B37" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="38" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H38" s="24"/>
+    </row>
+    <row r="39" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="43"/>
+      <c r="B39" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H39" s="40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="43"/>
+      <c r="B40" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="E40" s="34"/>
+      <c r="F40" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="H40" s="39" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="9"/>
+      <c r="E41" s="3"/>
+      <c r="G41" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="A24:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A17"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="92" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>